<commit_message>
Add log for company.py
</commit_message>
<xml_diff>
--- a/rasm.io.crawler/repository/suppliers.xlsx
+++ b/rasm.io.crawler/repository/suppliers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\rasm.io\rasm.io.crawler\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79ED6D0-CD3D-48B0-93D3-88AFC632EDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59548A5-631F-46FF-B46A-88357AEE2B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{E4CC4BC5-A6D4-43D8-B2E8-78E0D8C2BE79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4CC4BC5-A6D4-43D8-B2E8-78E0D8C2BE79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="323">
   <si>
     <t>Name</t>
   </si>
@@ -70,42 +64,6 @@
     <t>تلفن</t>
   </si>
   <si>
-    <t>شرکت بازرگانی بین المللی رایحه ماهریس</t>
-  </si>
-  <si>
-    <t>شرکت ایستا صنعت الکا</t>
-  </si>
-  <si>
-    <t>دنیای فرش یاقوت</t>
-  </si>
-  <si>
-    <t>شرکت خانمان</t>
-  </si>
-  <si>
-    <t>ابتین شیمی داود نوری</t>
-  </si>
-  <si>
-    <t>صنایع پزشکی آسیا تجهیز</t>
-  </si>
-  <si>
-    <t>زرین بایگان</t>
-  </si>
-  <si>
-    <t>شرکت نیوشا نیک</t>
-  </si>
-  <si>
-    <t>شرکت نگرش تحلیل سیستم ها</t>
-  </si>
-  <si>
-    <t>شرکت خاوران صنعت پاسارگاد</t>
-  </si>
-  <si>
-    <t>انبارسنگ اصفهان مرمر</t>
-  </si>
-  <si>
-    <t>شرکت استیل پاسارگاد</t>
-  </si>
-  <si>
     <t>شرکت پارس اکسید (شرکت بامسئولیت محدود)</t>
   </si>
   <si>
@@ -134,19 +92,929 @@
   </si>
   <si>
     <t>منطقه 13 ، شهرستان تهران ، بخش مرکزی ، شهر تهران، محله سلسبیل شمالی ، کوچه مسعود ، خیابان آزادی ، پلاک 274 ، طبقه سوم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کوشا فرآور گيتي  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">کشت و صنعت شکوه طعام وارنا  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">هواپيمايي قطر  شرکت </t>
+  </si>
+  <si>
+    <t>دانشگاه ازاد اسلامي واحد علوم تحقيقات دانشگاه</t>
+  </si>
+  <si>
+    <t>شرکت نفت پارس</t>
+  </si>
+  <si>
+    <t>شرکت پيشتازان تغذيه متين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ايران چوگل  </t>
+  </si>
+  <si>
+    <t>شرکت پاپيتال</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توليدي خوشخواب  </t>
+  </si>
+  <si>
+    <t>شرکت ايران خودرو ديزل</t>
+  </si>
+  <si>
+    <t>بيمارستان قلب تهران</t>
+  </si>
+  <si>
+    <t>شرکت سايپا ديزل</t>
+  </si>
+  <si>
+    <t>شرکت ملي گاز ايران</t>
+  </si>
+  <si>
+    <t>شرکت نفت بهران</t>
+  </si>
+  <si>
+    <t>موسسه فرهنگي انتشاراتي آگه سازان سبز</t>
+  </si>
+  <si>
+    <t>جهان رايانه كوثر شركت</t>
+  </si>
+  <si>
+    <t>موسسه خدمات تامين اقلام مصرفي کارکنان ناجا  موسسه خدمات تامين اقلام مصرفي کارکنان ناجا</t>
+  </si>
+  <si>
+    <t>شرکت نورد و توليد قطعات فولادي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کميته امداد امام خميني ره  </t>
+  </si>
+  <si>
+    <t>شركت توليدي و شيميايي  تولي پرس (سهامي عام)</t>
+  </si>
+  <si>
+    <t>شرکت ليکا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت ماشين سازي پارس </t>
+  </si>
+  <si>
+    <t>شرکت کيسون</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شركت صنعتي و بازرگاني صحت          </t>
+  </si>
+  <si>
+    <t>شرکت  کشت و صنعت شريف آباد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پارس برچسب  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت شيميايي دامت   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت پوشاتکس  </t>
+  </si>
+  <si>
+    <t>شرکت رزينفام</t>
+  </si>
+  <si>
+    <t>بانک ملت شرکتي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت الکترونيک افزار آزما </t>
+  </si>
+  <si>
+    <t>شرکت عطرآگين</t>
+  </si>
+  <si>
+    <t>هتل هويزه هتل هويزه</t>
+  </si>
+  <si>
+    <t>شرکت پارس حيان</t>
+  </si>
+  <si>
+    <t>موکت همدان شرکت موکت همدان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قاسم ايران  </t>
+  </si>
+  <si>
+    <t>شرکت تناوب</t>
+  </si>
+  <si>
+    <t>بيمارستان لقمان حکيم</t>
+  </si>
+  <si>
+    <t>تعاوني مصرف  کارکنان مرکز پزشکي شهيد مدرس</t>
+  </si>
+  <si>
+    <t>شرکت لابراتوار اخوي</t>
+  </si>
+  <si>
+    <t>شرکت کندر</t>
+  </si>
+  <si>
+    <t>شرکت ايران دلکو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شركت بازرگاني معادن وفلزات غيرآهني  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">کد ايران  </t>
+  </si>
+  <si>
+    <t>شرکت مسکن گستر</t>
+  </si>
+  <si>
+    <t>شرکت بازرگاني پيشرو سياحت گوشتيران</t>
+  </si>
+  <si>
+    <t>شرکت مهندسي فکور صنعت تهران</t>
+  </si>
+  <si>
+    <t>شرکت پتران</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت تعاوني ژاله نور  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت  مهندسي پارس نهند </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> توسعه و نگهداري اماکن ورزشي کشور  شرکت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شيميايي آذر آسا  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت لابراتور هاي داروهاي گياهي طبيعت زنده   </t>
+  </si>
+  <si>
+    <t>شرکت ملي مناطق نفت خير جنوب</t>
+  </si>
+  <si>
+    <t>شرکت نفت فلات قاره ايران</t>
+  </si>
+  <si>
+    <t>شرکت بهره برداري نفت و گاز مسجد سليمان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توليدي شکوفه شيرين بهار شرکت </t>
+  </si>
+  <si>
+    <t>لطيف گستر ديبا</t>
+  </si>
+  <si>
+    <t>شرکت نقش گوهر رهنورد</t>
+  </si>
+  <si>
+    <t>شرکت ياس دارو</t>
+  </si>
+  <si>
+    <t>شرکت انتقال گاز ايران</t>
+  </si>
+  <si>
+    <t>شرکت آذر کاوين</t>
+  </si>
+  <si>
+    <t>حلوا شکري عقاب</t>
+  </si>
+  <si>
+    <t>شهاب توشه شهاب توشه</t>
+  </si>
+  <si>
+    <t>شرکت بازرگاني حاميان اميد فردا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت  نام آور به شير </t>
+  </si>
+  <si>
+    <t>شرکت مهندسين مشاور صحن بوستان</t>
+  </si>
+  <si>
+    <t>شرکت  نويد رنگ پدارم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت دارو در مان سلفچگان    </t>
+  </si>
+  <si>
+    <t>شرکت دياموند پلور شرکت دياموند پلور</t>
+  </si>
+  <si>
+    <t>نخل تغذيه جنوب بيمارستان خاتم الانبيا</t>
+  </si>
+  <si>
+    <t>بازرگاني و صنايع  غذايي سبزدانه هرمزان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت شيميايي آرا فرايند  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. شركت پيمان شفق الوند </t>
+  </si>
+  <si>
+    <t>شرکت ساختماني و معدني صبا فتح</t>
+  </si>
+  <si>
+    <t>نفت ايرانول</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. شرکت گسترش و توسعه تحقيقات  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بهمن موتور شرکت </t>
+  </si>
+  <si>
+    <t>شرکت مهندسي تعميرات اساسي هواپيمايي فارس كوه</t>
+  </si>
+  <si>
+    <t>شرکت  خشکبار پردازان</t>
+  </si>
+  <si>
+    <t>شركت رسانه ساز دانش</t>
+  </si>
+  <si>
+    <t>پرستوي آبي ارگ پرستوي آبي ارگ</t>
+  </si>
+  <si>
+    <t>شركت توسعه تجارت و توليدي قند فيروزكوه-شكر</t>
+  </si>
+  <si>
+    <t>شرکت لوح فشرده پرتوآبي</t>
+  </si>
+  <si>
+    <t>شرکت روغن فوکس ايرانيان شرکت روغن فوکس ايرانيان</t>
+  </si>
+  <si>
+    <t>سي تو کار شرکت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پوياب فلز  </t>
+  </si>
+  <si>
+    <t>شرکت ديزل بندر جنوب</t>
+  </si>
+  <si>
+    <t>شرکت آني نام آوران امروز</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت بازرگاني آروين ارس  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">داروسازي توليد دارو    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تامين اجراي پارس برنا   </t>
+  </si>
+  <si>
+    <t>بانک پاسارگاد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت زيست دارو دانش </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت بنيان نوين شيمي پارس    </t>
+  </si>
+  <si>
+    <t>شركت پارند رستار</t>
+  </si>
+  <si>
+    <t>شرکت پاک بوم شيراز</t>
+  </si>
+  <si>
+    <t>شرکت هويک پارس</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت پارس ايده سبز  </t>
+  </si>
+  <si>
+    <t>صنايع غذايي چاشت آشام اميد سعيدي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توسعه الکترونيک گردو شهميرزاد شرکت </t>
+  </si>
+  <si>
+    <t>شرکت کيميا پژوهان خاور شيمي</t>
+  </si>
+  <si>
+    <t>بنياد نيکو کاري دستهاي مهربان بنياد نيکو کاري دستهاي مهربان</t>
+  </si>
+  <si>
+    <t>شرکت الفباي ايده برتر</t>
+  </si>
+  <si>
+    <t>توزيع دارويي  پورا پخش</t>
+  </si>
+  <si>
+    <t>. شركت توليدي لوح فشرده قرن 21</t>
+  </si>
+  <si>
+    <t>شرکت ايفا سرام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مانا بهداشت پارس   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. شرکت بوته سبز مهر آيين </t>
+  </si>
+  <si>
+    <t>شرکت  آتيه سازان تاسيسات ايرانيان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مهندسي بسپار گستر آريا  </t>
+  </si>
+  <si>
+    <t>فناپ شركت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مهان سپهر تابان  </t>
+  </si>
+  <si>
+    <t>شرکت صنايع آتش بس پارس</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سروش طراوت طبيعت    </t>
+  </si>
+  <si>
+    <t>شرکت گلشو پاک مهر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت سوت ايچ تبريز ( با مسئوليت محدود )  ( با مسئوليت محدود ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعاوني 749 مواد شوينده  </t>
+  </si>
+  <si>
+    <t>شرکت آذر مرجان (تبريز) شرکت آذر مرجان (تبريز)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آذر روان ساز  </t>
+  </si>
+  <si>
+    <t>شرکت آنيل طب آذران شرکت آنيل طب آذران</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نسترن فريدون شهر  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">گروه صنعتي جهان صادرات  </t>
+  </si>
+  <si>
+    <t>شرکت  نساجي کاشان</t>
+  </si>
+  <si>
+    <t>شرکت ايمن تاش سپاهان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت روغن نباتي ناز اصفهان  شرکت روغن نباتي ناز اصفهان </t>
+  </si>
+  <si>
+    <t>سازمان پاکيان کوير</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت مهرتاش سپاهان   </t>
+  </si>
+  <si>
+    <t>بازرگاني بنيان کار اسپادانا</t>
+  </si>
+  <si>
+    <t>شرکت روانکاران احياء سپاهان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت کيميا فرايند اسپيروز  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت مهندسي بازرگاني هفت آسمان  </t>
+  </si>
+  <si>
+    <t>شرکت  فراگام پتروفناورپويا</t>
+  </si>
+  <si>
+    <t>شرکت  پليمر آريا ساسول</t>
+  </si>
+  <si>
+    <t>بانک ايران-ونزوئلا</t>
+  </si>
+  <si>
+    <t>پيشگامان خوراک تابان شرکت سايپا يدک</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تبيان جراح  </t>
+  </si>
+  <si>
+    <t>شرکت کيميا اکسير اسيا</t>
+  </si>
+  <si>
+    <t>شرکت پاک آفرند سبز نوين</t>
+  </si>
+  <si>
+    <t>بانک ايران زمين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کامل برچسب پرند  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بهنام طب ايرانيان  </t>
+  </si>
+  <si>
+    <t>شرکت  آرسان تجارت آبا ريس</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت کيمياگران نيکي رسان  شرکت کيمياگران نيکي رسان </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت فراسوي انديشه توانا  شرکت فراسوي انديشه توانا </t>
+  </si>
+  <si>
+    <t>شرکت شرکت کيان البرز زرين(اراک)</t>
+  </si>
+  <si>
+    <t>مهراقتصاد بانک</t>
+  </si>
+  <si>
+    <t>شرکت  پشتيباني توليدي ايده آل فاتک</t>
+  </si>
+  <si>
+    <t>شرکت  کف ساز شرق</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سيمان زاوه تربت  </t>
+  </si>
+  <si>
+    <t>مشاور نرم افزار محك شركت</t>
+  </si>
+  <si>
+    <t>شرکت آرمينا گستران شرق شرکت آرمينا گستران شرق</t>
+  </si>
+  <si>
+    <t>شرکت کيميا کوشا تجارت (خوزستان) شرکت کيميا کوشا تجارت (خوزستان)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توليدي شادن زنجان  </t>
+  </si>
+  <si>
+    <t>شرکت حامد راه ماندگار</t>
+  </si>
+  <si>
+    <t>توليدي پالنده صاف</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعاوني توليدي نازگل سرحد  </t>
+  </si>
+  <si>
+    <t>شرکت واچين کومش سمنان</t>
+  </si>
+  <si>
+    <t>شرکت رنگين کمان هيرمند</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رزين سازان فارس  </t>
+  </si>
+  <si>
+    <t>شرکت ماهان دشت پارسيان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ايمن پاليز مهار  </t>
+  </si>
+  <si>
+    <t>بازرگاني هوداد آريا</t>
+  </si>
+  <si>
+    <t>. موسسه خانه فردوسيان جوان قم</t>
+  </si>
+  <si>
+    <t>شرکت مداوا گستر آبيدر</t>
+  </si>
+  <si>
+    <t>شرکت سلامت گستر ويشاد</t>
+  </si>
+  <si>
+    <t>شرکت سفيد بام کرمانيان شرکت سفيد بام کرمانيان</t>
+  </si>
+  <si>
+    <t>شرکت چيني کرد</t>
+  </si>
+  <si>
+    <t>شرکت  کيميا فرآيند بيستون</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساينا سلامت پارس  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت  پاک پويان زاگرس </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت داروسازي نياک  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت  نصر نوين گلستان </t>
+  </si>
+  <si>
+    <t>پخش آريا پويا گلستان</t>
+  </si>
+  <si>
+    <t>بيمارستان مطهري بيمارستان مطهري</t>
+  </si>
+  <si>
+    <t>شرکت سلامت گستر سانيار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت کيميا کاران شيما  </t>
+  </si>
+  <si>
+    <t>شرکت  سوليکو کاله</t>
+  </si>
+  <si>
+    <t>لابراتوار گلپسند</t>
+  </si>
+  <si>
+    <t>آذر گستر  ساحل</t>
+  </si>
+  <si>
+    <t>شرکت  بهار شور</t>
+  </si>
+  <si>
+    <t>صنعتگران روغن گيل توحيد صنعتگران روغن گيل توحيد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بهار پويان سپاهان  </t>
+  </si>
+  <si>
+    <t>شرکت سيماب رزين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">توسعه و بهبود نهادهاي کشاورزي پارس يزد  </t>
+  </si>
+  <si>
+    <t>شرکت گيله دام کاسپين شرکت گيله دام کاسپين</t>
+  </si>
+  <si>
+    <t xml:space="preserve">روانکاران نوين انديش پايدار  </t>
+  </si>
+  <si>
+    <t>شرکت داروسازي دانا</t>
+  </si>
+  <si>
+    <t>بيمارستان فيروزگر (شرکت نوين واران) جهان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">به رشد کوير رفسنجان  </t>
+  </si>
+  <si>
+    <t>شرکت  عمران آذرستان</t>
+  </si>
+  <si>
+    <t>دانشگاه اميرکبير شرکت افق ماندگار جنوب (پروژه اميرکبير)</t>
+  </si>
+  <si>
+    <t>شرکت ظريف کار امين بيمارستان مصطفي خميني</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سلولزي حرير پارسيان  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شيما گرو يزد  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نرمينه گستر نطنز  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">گيلان سويا  </t>
+  </si>
+  <si>
+    <t>شرکت ديريلينگ اينترنشنال ليميتد</t>
+  </si>
+  <si>
+    <t>شرکت سمبل شيمي</t>
+  </si>
+  <si>
+    <t>برنا گستران نيك پارسه ب</t>
+  </si>
+  <si>
+    <t>شرکت آرايشي سورينت کيش</t>
+  </si>
+  <si>
+    <t>موسسه خيريه آموزشي پژوهشي درماني پيوند اعضاء ابوعلي سينا</t>
+  </si>
+  <si>
+    <t>سازمان ياتا اکسپرس</t>
+  </si>
+  <si>
+    <t>مهيار مس رفسنجان مهيار مس رفسنجان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پارس کرپ  </t>
+  </si>
+  <si>
+    <t>بانک صادرات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت فن آوران کارزا  </t>
+  </si>
+  <si>
+    <t>شرکت اميد خادم بيمارستان ميلاد</t>
+  </si>
+  <si>
+    <t>اسپيدار سبز SS</t>
+  </si>
+  <si>
+    <t>شرکت زرين پلاستيک نيلگون</t>
+  </si>
+  <si>
+    <t>رجب  محمد رازي</t>
+  </si>
+  <si>
+    <t>شرکت تعاوني توليدي و توزيعي بنيان اعتماد طوس</t>
+  </si>
+  <si>
+    <t>شرکت درين سيالات حفاري</t>
+  </si>
+  <si>
+    <t>شرکت  سازمان اوقاف</t>
+  </si>
+  <si>
+    <t>سازمان تامين اجتماعي</t>
+  </si>
+  <si>
+    <t>سازمان هلال احمر تهران سازمان هلال احمر تهران</t>
+  </si>
+  <si>
+    <t>شهرداري ابهر</t>
+  </si>
+  <si>
+    <t>شهرداري سجاس</t>
+  </si>
+  <si>
+    <t>شهرداري  صائين قلعه</t>
+  </si>
+  <si>
+    <t>صندوق بازنشستگي کشور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شركت سازمان ملي استاندارد ايران/ اداره كل استاندارد استان خراسان جنوبي </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شركت سازمان ملي استاندارد ايران </t>
+  </si>
+  <si>
+    <t>تبريز دانشگاه علوم پزشکي</t>
+  </si>
+  <si>
+    <t>دبيرستان  حرابن رياحي</t>
+  </si>
+  <si>
+    <t>دبيرستان ابو علي سينا دبيرستان ابو علي سينا</t>
+  </si>
+  <si>
+    <t>نگاه پردازان امين سيما کيش شرکت</t>
+  </si>
+  <si>
+    <t>شرکت مستقل تجارت منطقه آزاد ماکو</t>
+  </si>
+  <si>
+    <t>کميته امداد امام خميني کميته</t>
+  </si>
+  <si>
+    <t>هواپيمايي ساها هواپيمايي ساها</t>
+  </si>
+  <si>
+    <t>بيمارستان  بقيه الله</t>
+  </si>
+  <si>
+    <t>وزارت دفاع و پشتيباني مجتمع هويزه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پاک سون نوين ارس  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نيروي انتظامي ناجا ( پليس آگاهي ) - 411435465457  </t>
+  </si>
+  <si>
+    <t>بنياد تعاون ستاد فرماندهي انتظامي استان اليرز بنياد تعاون ستاد فرماندهي انتظامي استان اليرز</t>
+  </si>
+  <si>
+    <t>وزارت دفاع و پشتيباني  نيروهاي مسلح(خاتم)</t>
+  </si>
+  <si>
+    <t>مرکز آموزشي درماني نمازي</t>
+  </si>
+  <si>
+    <t>دهيار قاسم آباد کوچک</t>
+  </si>
+  <si>
+    <t>شرکت چهره سازان موژان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آريستا سرام آريا  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">گروه شرکتهاي توليدي و بازرگاني شانلي  گروه شرکتهاي توليدي و بازرگاني شانلي </t>
+  </si>
+  <si>
+    <t>معاونت آمادوپشتيباني سپاه</t>
+  </si>
+  <si>
+    <t>وزارت دفاع و پشتيباني نيروهاي مسلح ( سپاه پاسداران )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> استاندارد البرز اداره کل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">درفام پرارين نوين  </t>
+  </si>
+  <si>
+    <t>شرکت تدارک هنر راهبردي نارون (تهران) شرکت تدارک هنر راهبردي نارون (تهران)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هومان بناي کادوس  </t>
+  </si>
+  <si>
+    <t>سرچشمه نيلگون سي سخت سرچشمه نيلگون سي سخت</t>
+  </si>
+  <si>
+    <t>شرکت گولدن آبشار</t>
+  </si>
+  <si>
+    <t>شرکت  چهره آراک</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آراد توسعه انرژي فيدار  </t>
+  </si>
+  <si>
+    <t>شرکت توسعه تجارت دالين سامان</t>
+  </si>
+  <si>
+    <t>مجتمع بيمارستاني امام خميني-ره</t>
+  </si>
+  <si>
+    <t>شرکت راهداري استان البرز</t>
+  </si>
+  <si>
+    <t>وزارت بهداشت و درمان و آموزش پزشکي</t>
+  </si>
+  <si>
+    <t>بيمارستان  شهيد اکبر آبادي</t>
+  </si>
+  <si>
+    <t>بيمارستان بيمارستان هاشمي نژاد</t>
+  </si>
+  <si>
+    <t>شرکت اسپينر تجارت ايزد دژ شرکت اسپينر تجارت ايزد دژ</t>
+  </si>
+  <si>
+    <t>شرکت خانه امن البرز ايرانيان</t>
+  </si>
+  <si>
+    <t>شرکت گيتي سلامت آريا</t>
+  </si>
+  <si>
+    <t>شرکت توسعه تجارت الکترونيک گلستان  (مديسه)</t>
+  </si>
+  <si>
+    <t>آريا سهند مهر آريا سهند مهر</t>
+  </si>
+  <si>
+    <t>فرمانداري تهران .</t>
+  </si>
+  <si>
+    <t>شوراي اسلامي شهر تنکمان</t>
+  </si>
+  <si>
+    <t>معاونت غذا و دارو</t>
+  </si>
+  <si>
+    <t>شرکت ابنيه تاسيسات هيراد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سلام تهران افرا توزيع </t>
+  </si>
+  <si>
+    <t>شرکت  نيک آئين حساب بندر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آروند سير نشاط رود  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">آترين صنعت پارسيان طب   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شرکت طلاي سياه مکران  </t>
+  </si>
+  <si>
+    <t>شرکت کاسپين درياي پهنه خزر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">طراحان ايده کارآمدان هخامنش  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">برچسب زرين نگار پاسارگاد  </t>
+  </si>
+  <si>
+    <t>شرکت آرشيدا سلامت آرايه</t>
+  </si>
+  <si>
+    <t>شرکت رامان فيدار سازه</t>
+  </si>
+  <si>
+    <t>شرکت فن آور سازان هوشمند پرديس</t>
+  </si>
+  <si>
+    <t>شرکت زرين پخش نوين جهان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تکميل منسوج آرمان گستر  </t>
+  </si>
+  <si>
+    <t>شرکت اوکسين داروي وشت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آيريا رسام خاورميانه  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">مشاوره مهندسي آرکا انديش فرا پارتاک  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">پاک حيات کيميا پارس  </t>
+  </si>
+  <si>
+    <t>ارزش آفريني غذايي جواهر دشت آويژه کاسپين</t>
+  </si>
+  <si>
+    <t>شرکت   بازرگاني پژواک سازه کردستان</t>
+  </si>
+  <si>
+    <t>شهرداري  فرديس</t>
+  </si>
+  <si>
+    <t>شرکت  تهران استون مهرآگين</t>
+  </si>
+  <si>
+    <t>شرکت پيشگامان توسعه تجارت رونيکا</t>
+  </si>
+  <si>
+    <t>شرکت به روز رسان فن آور بين الملل شرکت به روز رسان فن آور بين الملل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ايده پردازان طرح و نقش صنعت پايدار قرن  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">شينا بهتاش آريافر  </t>
+  </si>
+  <si>
+    <t>شرکت  پيشروان پاك ماهور گيتي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">نرمين تجارت پارسه  </t>
+  </si>
+  <si>
+    <t>شرکت شهر پروتئين محراب قائم</t>
+  </si>
+  <si>
+    <t>شرکت بازرگاني اميد اخباراتي شرکت بازرگاني اميد اخباراتي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پويا انديش باران  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">طلايه گستران شاه رنگ  </t>
+  </si>
+  <si>
+    <t>شرکت گيتا تجارت سرمد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مهام شيمي اميد اروند  </t>
+  </si>
+  <si>
+    <t>خدمات خودرويي ساميا شرکت</t>
+  </si>
+  <si>
+    <t>شرکت سيما رخ رازي</t>
+  </si>
+  <si>
+    <t>شرکت نادين صنعت پاک</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -169,8 +1037,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +1068,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006400"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99C2ED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,31 +1162,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="MDSBadStyle" xfId="3" xr:uid="{73BD706C-489A-405F-B965-140902C5572E}"/>
+    <cellStyle name="MDSHeader" xfId="9" xr:uid="{DFD514C5-3895-4217-A7D6-063762CC067C}"/>
+    <cellStyle name="MDSInputStyle" xfId="4" xr:uid="{DE46D672-AB34-4C19-A75C-FC164F48296B}"/>
+    <cellStyle name="MDSNewRecord" xfId="6" xr:uid="{52BAA245-64E9-4BC9-B9E7-46C50457FDF0}"/>
+    <cellStyle name="MDSNonPivot" xfId="8" xr:uid="{F0B04646-DE38-409A-9BEF-7FAE8E1D62AC}"/>
+    <cellStyle name="MDSNormal" xfId="2" xr:uid="{4BED7F51-B872-4BB1-8C50-7928506C6FAF}"/>
+    <cellStyle name="MDSReadOnlyStyle" xfId="5" xr:uid="{7800E35B-F71C-4787-AF17-F2AE92EDD6CD}"/>
+    <cellStyle name="MDSUnmanaged" xfId="7" xr:uid="{608C67F8-0ACB-4F5D-BBB7-B0BA5CC1A573}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{A3363707-BB7B-4E4C-BF3E-484A9F3BCDC6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -574,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB4CC9-1D68-4A2B-8047-06D8A0E18E0F}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,99 +1575,1510 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1">
-        <v>26755</v>
+      <c r="A2" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1">
-        <v>26754</v>
+      <c r="A3" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1">
-        <v>26753</v>
+      <c r="A4" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1">
-        <v>26751</v>
+      <c r="A5" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1">
-        <v>26750</v>
+      <c r="A6" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1">
-        <v>26749</v>
+      <c r="A7" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>26748</v>
+      <c r="A8" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1">
-        <v>26746</v>
+      <c r="A9" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1">
-        <v>26744</v>
+      <c r="A10" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1">
-        <v>26743</v>
+      <c r="A11" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="5">
-        <v>26742</v>
-      </c>
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="5">
-        <v>26741</v>
+      <c r="A13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="8" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -789,31 +3147,31 @@
         <v>10101426979</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>98691</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I2" s="7">
         <v>1111111111</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -824,31 +3182,31 @@
         <v>14006673353</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>507732</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>1345616555</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>